<commit_message>
Changed dataset since a company changed their ticker
</commit_message>
<xml_diff>
--- a/datasets/profit_earnings.xlsx
+++ b/datasets/profit_earnings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ali_ahad/Desktop/rmsc4002/part1/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91A6434-6C74-0C44-9687-1834C6C3BCC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B5DF4F-2782-9146-BC24-EC8D98BF4948}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,12 +44,6 @@
   </si>
   <si>
     <t>SPPJY</t>
-  </si>
-  <si>
-    <t>PolyOne</t>
-  </si>
-  <si>
-    <t>POL</t>
   </si>
   <si>
     <t>Avient</t>
@@ -338,6 +332,12 @@
   </si>
   <si>
     <t>HUN</t>
+  </si>
+  <si>
+    <t>Svenska Cellulosa</t>
+  </si>
+  <si>
+    <t>SVCBY</t>
   </si>
 </sst>
 </file>
@@ -717,10 +717,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -804,7 +804,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="4">
-        <v>4.3899999999999997</v>
+        <v>4.57</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -838,7 +838,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="4">
-        <v>4.57</v>
+        <v>4.6399999999999997</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -866,13 +866,13 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C5" s="4">
-        <v>4.6399999999999997</v>
+        <v>5.68</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -899,14 +899,14 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="4">
-        <v>5.68</v>
+      <c r="C6" s="2">
+        <v>7.15</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -933,9 +933,6 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1061,6 +1058,9 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -1086,9 +1086,6 @@
       <c r="Z12" s="2"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -1214,6 +1211,9 @@
       <c r="Z17" s="2"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -1239,9 +1239,6 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -1367,6 +1364,9 @@
       <c r="Z23" s="2"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -1392,9 +1392,6 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -1520,6 +1517,9 @@
       <c r="Z29" s="2"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -1545,9 +1545,6 @@
       <c r="Z30" s="2"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -1673,6 +1670,9 @@
       <c r="Z35" s="2"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -1698,9 +1698,6 @@
       <c r="Z36" s="2"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -1826,6 +1823,9 @@
       <c r="Z41" s="2"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
@@ -1851,9 +1851,6 @@
       <c r="Z42" s="2"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
@@ -2028,7 +2025,7 @@
       <c r="Y49" s="2"/>
       <c r="Z49" s="2"/>
     </row>
-    <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
@@ -2104,6 +2101,9 @@
       <c r="Z52" s="2"/>
     </row>
     <row r="53" spans="1:26" ht="13" x14ac:dyDescent="0.15">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
@@ -2129,9 +2129,6 @@
       <c r="Z53" s="2"/>
     </row>
     <row r="54" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
@@ -2257,6 +2254,9 @@
       <c r="Z58" s="2"/>
     </row>
     <row r="59" spans="1:26" ht="13" x14ac:dyDescent="0.15">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
@@ -28573,34 +28573,6 @@
       <c r="Y998" s="2"/>
       <c r="Z998" s="2"/>
     </row>
-    <row r="999" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A999" s="2"/>
-      <c r="B999" s="2"/>
-      <c r="C999" s="2"/>
-      <c r="D999" s="2"/>
-      <c r="E999" s="2"/>
-      <c r="F999" s="2"/>
-      <c r="G999" s="2"/>
-      <c r="H999" s="2"/>
-      <c r="I999" s="2"/>
-      <c r="J999" s="2"/>
-      <c r="K999" s="2"/>
-      <c r="L999" s="2"/>
-      <c r="M999" s="2"/>
-      <c r="N999" s="2"/>
-      <c r="O999" s="2"/>
-      <c r="P999" s="2"/>
-      <c r="Q999" s="2"/>
-      <c r="R999" s="2"/>
-      <c r="S999" s="2"/>
-      <c r="T999" s="2"/>
-      <c r="U999" s="2"/>
-      <c r="V999" s="2"/>
-      <c r="W999" s="2"/>
-      <c r="X999" s="2"/>
-      <c r="Y999" s="2"/>
-      <c r="Z999" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28630,10 +28602,10 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C2" s="4">
         <v>2.04</v>
@@ -28641,10 +28613,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C3" s="4">
         <v>4.43</v>
@@ -28652,10 +28624,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C4" s="4">
         <v>5.24</v>
@@ -28663,10 +28635,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C5" s="4">
         <v>6.08</v>
@@ -28674,10 +28646,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C6" s="4">
         <v>6.1</v>
@@ -28712,10 +28684,10 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" s="4">
         <v>3.16</v>
@@ -28723,10 +28695,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="4">
         <v>3.44</v>
@@ -28734,10 +28706,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4">
         <v>3.5</v>
@@ -28745,10 +28717,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4">
         <v>3.73</v>
@@ -28756,10 +28728,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="4">
         <v>4.0199999999999996</v>
@@ -28794,10 +28766,10 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="4">
         <v>1.1399999999999999</v>
@@ -28805,10 +28777,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="4">
         <v>1.18</v>
@@ -28816,10 +28788,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4" s="4">
         <v>2.67</v>
@@ -28827,10 +28799,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5" s="4">
         <v>2.97</v>
@@ -28838,10 +28810,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" s="4">
         <v>4.57</v>
@@ -28876,10 +28848,10 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="4">
         <v>4.8499999999999996</v>
@@ -28887,10 +28859,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" s="4">
         <v>6</v>
@@ -28898,10 +28870,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" s="4">
         <v>7.09</v>
@@ -28909,10 +28881,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C5" s="4">
         <v>7.86</v>
@@ -28920,10 +28892,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" s="4">
         <v>7.91</v>
@@ -28958,10 +28930,10 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" s="4">
         <v>1.83</v>
@@ -28969,10 +28941,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C3" s="4">
         <v>2.0499999999999998</v>
@@ -28980,10 +28952,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" s="4">
         <v>3.35</v>
@@ -28991,10 +28963,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" s="4">
         <v>4.0599999999999996</v>
@@ -29002,10 +28974,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C6" s="4">
         <v>4.2</v>
@@ -29040,10 +29012,10 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2" s="4">
         <v>1.29</v>
@@ -29051,10 +29023,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C3" s="4">
         <v>1.3</v>
@@ -29062,10 +29034,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C4" s="4">
         <v>1.49</v>
@@ -29073,10 +29045,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C5" s="4">
         <v>1.65</v>
@@ -29084,10 +29056,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C6" s="4">
         <v>2.35</v>
@@ -29122,10 +29094,10 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" s="4">
         <v>1.27</v>
@@ -29133,10 +29105,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3" s="4">
         <v>3.84</v>
@@ -29144,10 +29116,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C4" s="4">
         <v>4.82</v>
@@ -29155,10 +29127,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C5" s="4">
         <v>4.92</v>
@@ -29166,10 +29138,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C6" s="4">
         <v>5.15</v>
@@ -29204,10 +29176,10 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C2" s="4">
         <v>0.9</v>
@@ -29215,10 +29187,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C3" s="4">
         <v>1.44</v>
@@ -29226,10 +29198,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C4" s="4">
         <v>5.53</v>
@@ -29237,10 +29209,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C5" s="4">
         <v>6.25</v>
@@ -29248,10 +29220,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C6" s="4">
         <v>6.7</v>
@@ -29286,10 +29258,10 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C2" s="4">
         <v>1.93</v>
@@ -29297,10 +29269,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C3" s="4">
         <v>2.41</v>
@@ -29308,10 +29280,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C4" s="4">
         <v>2.59</v>
@@ -29319,10 +29291,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C5" s="4">
         <v>2.98</v>
@@ -29330,10 +29302,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C6" s="4">
         <v>3.5</v>

</xml_diff>